<commit_message>
economic value of image memorability v2
</commit_message>
<xml_diff>
--- a/study1_2/data/output/bubble_plot_data.xlsx
+++ b/study1_2/data/output/bubble_plot_data.xlsx
@@ -1,102 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
-  <si>
-    <t>group</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>memory_score</t>
-  </si>
-  <si>
-    <t>sd</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>percentage</t>
-  </si>
-  <si>
-    <t>se</t>
-  </si>
-  <si>
-    <t>ci_lower</t>
-  </si>
-  <si>
-    <t>ci_upper</t>
-  </si>
-  <si>
-    <t>All businesses</t>
-  </si>
-  <si>
-    <t>Restaurants</t>
-  </si>
-  <si>
-    <t>Drinks</t>
-  </si>
-  <si>
-    <t>drink</t>
-  </si>
-  <si>
-    <t>food</t>
-  </si>
-  <si>
-    <t>inside</t>
-  </si>
-  <si>
-    <t>menu</t>
-  </si>
-  <si>
-    <t>outside</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -104,36 +42,85 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -421,478 +408,562 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>group</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>memory_score</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sd</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>percentage</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>se</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>ci_lower</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>ci_upper</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>All businesses</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>drink</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>0.8309115309641626</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>0.07227451023121721</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>13338</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="n">
         <v>8.608215818516248</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="n">
         <v>0.0006258061125744033</v>
       </c>
-      <c r="H2">
+      <c r="H2" t="n">
         <v>0.8296849509835168</v>
       </c>
-      <c r="I2">
+      <c r="I2" t="n">
         <v>0.8321381109448084</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>All businesses</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>0.7882749209793839</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>0.08175965784027163</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>84788</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="n">
         <v>54.72135273806835</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="n">
         <v>0.0002807836852028521</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="n">
         <v>0.7877245849563863</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="n">
         <v>0.7888252570023815</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>All businesses</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>0.6687294282054268</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="n">
         <v>0.09972819208823439</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="n">
         <v>42935</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="n">
         <v>27.7098325212172</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="n">
         <v>0.0004812959558002797</v>
       </c>
-      <c r="H4">
+      <c r="H4" t="n">
         <v>0.6677860881320583</v>
       </c>
-      <c r="I4">
+      <c r="I4" t="n">
         <v>0.6696727682787953</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>All businesses</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>0.8261441441441442</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="n">
         <v>0.06892039818380968</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="n">
         <v>999</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="n">
         <v>0.6447449094840104</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="n">
         <v>0.002180544900220299</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="n">
         <v>0.8218702761397124</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="n">
         <v>0.8304180121485759</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6">
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>All businesses</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>0.6909572370974001</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="n">
         <v>0.1027183370728225</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="n">
         <v>12885</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="n">
         <v>8.315854012714189</v>
       </c>
-      <c r="G6">
+      <c r="G6" t="n">
         <v>0.0009049107936750363</v>
       </c>
-      <c r="H6">
+      <c r="H6" t="n">
         <v>0.689183611941797</v>
       </c>
-      <c r="I6">
+      <c r="I6" t="n">
         <v>0.6927308622530032</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7">
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Restaurants</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>drink</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
         <v>0.8261828243056295</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="n">
         <v>0.07421027239064132</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="n">
         <v>9397</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="n">
         <v>7.139275512064669</v>
       </c>
-      <c r="G7">
+      <c r="G7" t="n">
         <v>0.0007655426871591472</v>
       </c>
-      <c r="H7">
+      <c r="H7" t="n">
         <v>0.8246823606387976</v>
       </c>
-      <c r="I7">
+      <c r="I7" t="n">
         <v>0.8276832879724614</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8">
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Restaurants</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
         <v>0.7835352000411395</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="n">
         <v>0.08100669821157072</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="n">
         <v>77784</v>
       </c>
-      <c r="F8">
+      <c r="F8" t="n">
         <v>59.09560566462043</v>
       </c>
-      <c r="G8">
+      <c r="G8" t="n">
         <v>0.0002904529518648382</v>
       </c>
-      <c r="H8">
+      <c r="H8" t="n">
         <v>0.7829659122554844</v>
       </c>
-      <c r="I8">
+      <c r="I8" t="n">
         <v>0.7841044878267946</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9">
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Restaurants</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
         <v>0.659903518490792</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="n">
         <v>0.09671306651497577</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="n">
         <v>33395</v>
       </c>
-      <c r="F9">
+      <c r="F9" t="n">
         <v>25.37151279401933</v>
       </c>
-      <c r="G9">
+      <c r="G9" t="n">
         <v>0.0005292299698374061</v>
       </c>
-      <c r="H9">
+      <c r="H9" t="n">
         <v>0.6588662277499107</v>
       </c>
-      <c r="I9">
+      <c r="I9" t="n">
         <v>0.6609408092316733</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10">
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Restaurants</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
         <v>0.8277076749435667</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="n">
         <v>0.06824309561575273</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="n">
         <v>886</v>
       </c>
-      <c r="F10">
+      <c r="F10" t="n">
         <v>0.6731295204521971</v>
       </c>
-      <c r="G10">
+      <c r="G10" t="n">
         <v>0.002292671635256885</v>
       </c>
-      <c r="H10">
+      <c r="H10" t="n">
         <v>0.8232140385384632</v>
       </c>
-      <c r="I10">
+      <c r="I10" t="n">
         <v>0.8322013113486701</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11">
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Restaurants</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
         <v>0.6885422160991931</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="n">
         <v>0.1034309616188728</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="n">
         <v>10162</v>
       </c>
-      <c r="F11">
+      <c r="F11" t="n">
         <v>7.720476508843372</v>
       </c>
-      <c r="G11">
+      <c r="G11" t="n">
         <v>0.001026032144891376</v>
       </c>
-      <c r="H11">
+      <c r="H11" t="n">
         <v>0.6865311930952059</v>
       </c>
-      <c r="I11">
+      <c r="I11" t="n">
         <v>0.6905532391031802</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12">
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Drinks</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>drink</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
         <v>0.8317269803837496</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="n">
         <v>0.07100373363929624</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="n">
         <v>9329</v>
       </c>
-      <c r="F12">
+      <c r="F12" t="n">
         <v>13.41375740495773</v>
       </c>
-      <c r="G12">
+      <c r="G12" t="n">
         <v>0.0007351291423301838</v>
       </c>
-      <c r="H12">
+      <c r="H12" t="n">
         <v>0.8302861272647825</v>
       </c>
-      <c r="I12">
+      <c r="I12" t="n">
         <v>0.8331678335027167</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13">
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Drinks</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
         <v>0.7824476224760284</v>
       </c>
-      <c r="D13">
+      <c r="D13" t="n">
         <v>0.08320603063379556</v>
       </c>
-      <c r="E13">
+      <c r="E13" t="n">
         <v>30557</v>
       </c>
-      <c r="F13">
+      <c r="F13" t="n">
         <v>43.93656179904526</v>
       </c>
-      <c r="G13">
+      <c r="G13" t="n">
         <v>0.0004759917738719854</v>
       </c>
-      <c r="H13">
+      <c r="H13" t="n">
         <v>0.7815146785992393</v>
       </c>
-      <c r="I13">
+      <c r="I13" t="n">
         <v>0.7833805663528175</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14">
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Drinks</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>inside</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
         <v>0.6627358686257563</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="n">
         <v>0.09901886499598749</v>
       </c>
-      <c r="E14">
+      <c r="E14" t="n">
         <v>23140</v>
       </c>
-      <c r="F14">
+      <c r="F14" t="n">
         <v>33.27198481624202</v>
       </c>
-      <c r="G14">
+      <c r="G14" t="n">
         <v>0.0006509329660077744</v>
       </c>
-      <c r="H14">
+      <c r="H14" t="n">
         <v>0.661460040012381</v>
       </c>
-      <c r="I14">
+      <c r="I14" t="n">
         <v>0.6640116972391316</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15">
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Drinks</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
         <v>0.8247185185185186</v>
       </c>
-      <c r="D15">
+      <c r="D15" t="n">
         <v>0.07257846404646723</v>
       </c>
-      <c r="E15">
+      <c r="E15" t="n">
         <v>405</v>
       </c>
-      <c r="F15">
+      <c r="F15" t="n">
         <v>0.5823316270777017</v>
       </c>
-      <c r="G15">
+      <c r="G15" t="n">
         <v>0.003606452873565004</v>
       </c>
-      <c r="H15">
+      <c r="H15" t="n">
         <v>0.8176498708863312</v>
       </c>
-      <c r="I15">
+      <c r="I15" t="n">
         <v>0.831787166150706</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16">
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Drinks</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>outside</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
         <v>0.6769328102010789</v>
       </c>
-      <c r="D16">
+      <c r="D16" t="n">
         <v>0.100619871947045</v>
       </c>
-      <c r="E16">
+      <c r="E16" t="n">
         <v>6117</v>
       </c>
-      <c r="F16">
+      <c r="F16" t="n">
         <v>8.795364352677288</v>
       </c>
-      <c r="G16">
+      <c r="G16" t="n">
         <v>0.001286514010141346</v>
       </c>
-      <c r="H16">
+      <c r="H16" t="n">
         <v>0.6744112427412018</v>
       </c>
-      <c r="I16">
+      <c r="I16" t="n">
         <v>0.679454377660956</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>